<commit_message>
Work Towards Getting Rays Working
Figured out how to get Rays to render.
Added new constructor to the Ray class.
Added Bounds property to Ray. It only reprisents a line segment of the
vector and location.
Added Intersections between Rays and other simple line types.
Added Intersections between Triangles and other simple line types.
Changed how lines and rays are called. You no longer need to add the
direction vector to the location.
Ticked off the current intersection types in checklist.
</commit_message>
<xml_diff>
--- a/Documents/Geometry.xlsx
+++ b/Documents/Geometry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19155" windowHeight="7245"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19155" windowHeight="7245" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="30">
   <si>
     <t>Point</t>
   </si>
@@ -88,6 +88,24 @@
   </si>
   <si>
     <t>Containinigs</t>
+  </si>
+  <si>
+    <t>Polygon Contour</t>
+  </si>
+  <si>
+    <t>Quadratic Bezier</t>
+  </si>
+  <si>
+    <t>Cubic Bezier</t>
+  </si>
+  <si>
+    <t>Circular Arc</t>
+  </si>
+  <si>
+    <t>Line Segment</t>
+  </si>
+  <si>
+    <t>Elliptical Arc</t>
   </si>
 </sst>
 </file>
@@ -180,18 +198,18 @@
   <tableColumns count="16">
     <tableColumn id="1" name="Intersectings"/>
     <tableColumn id="2" name="Point"/>
+    <tableColumn id="5" name="Line Segment"/>
+    <tableColumn id="3" name="Ray"/>
     <tableColumn id="4" name="Line"/>
-    <tableColumn id="3" name="Ray"/>
-    <tableColumn id="5" name="LineSegment"/>
+    <tableColumn id="12" name="Quadratic Bezier"/>
+    <tableColumn id="13" name="Cubic Bezier"/>
     <tableColumn id="6" name="Triangle"/>
+    <tableColumn id="8" name="Circle"/>
+    <tableColumn id="9" name="Circular Arc"/>
+    <tableColumn id="10" name="Ellipse"/>
+    <tableColumn id="11" name="Elliptical Arc"/>
     <tableColumn id="7" name="Rectangle"/>
-    <tableColumn id="8" name="Circle"/>
-    <tableColumn id="9" name="CircularArc"/>
-    <tableColumn id="10" name="Ellipse"/>
-    <tableColumn id="11" name="EllipticalArc"/>
-    <tableColumn id="12" name="QuadraticBezier"/>
-    <tableColumn id="13" name="CubicBezier"/>
-    <tableColumn id="14" name="Polygon"/>
+    <tableColumn id="14" name="Polygon Contour"/>
     <tableColumn id="15" name="Polyline"/>
     <tableColumn id="16" name="Path"/>
   </tableColumns>
@@ -511,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -521,7 +539,7 @@
     <col min="2" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="64.5">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="63.75">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -910,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -920,7 +938,7 @@
     <col min="2" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="65.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="66.75">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -928,40 +946,40 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>14</v>
@@ -978,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1022,46 +1040,46 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -1078,13 +1096,13 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1093,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -1108,10 +1126,10 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -1122,46 +1140,46 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -1172,46 +1190,46 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -1222,22 +1240,22 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1246,22 +1264,22 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -1272,19 +1290,19 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1322,46 +1340,46 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -1372,19 +1390,19 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1422,46 +1440,46 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -1472,19 +1490,19 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1522,46 +1540,46 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -1572,46 +1590,46 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -1722,7 +1740,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:P16">
-    <cfRule type="iconSet" priority="2">
+    <cfRule type="iconSet" priority="10">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>

</xml_diff>

<commit_message>
More Ray and Triangle Intersection Methods
Updating to latest VS 2017 Preview.
Adding untested missing Ray intersection methods.
Adding some of the remaining missing Triangle intersection methods.
</commit_message>
<xml_diff>
--- a/Documents/Geometry.xlsx
+++ b/Documents/Geometry.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19155" windowHeight="7245" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19155" windowHeight="7245" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="3" r:id="rId1"/>
-    <sheet name="Intersectings" sheetId="1" r:id="rId2"/>
-    <sheet name="Intersections" sheetId="2" r:id="rId3"/>
+    <sheet name="Contains" sheetId="4" r:id="rId2"/>
+    <sheet name="Intersects" sheetId="1" r:id="rId3"/>
+    <sheet name="Intersection" sheetId="2" r:id="rId4"/>
+    <sheet name="Scan-beam" sheetId="5" r:id="rId5"/>
+    <sheet name="Scan-beam Left" sheetId="6" r:id="rId6"/>
+    <sheet name="Scan-Beam Right" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="30">
   <si>
     <t>Point</t>
   </si>
@@ -78,16 +82,7 @@
     <t>Length</t>
   </si>
   <si>
-    <t>Intersections</t>
-  </si>
-  <si>
     <t>Properties</t>
-  </si>
-  <si>
-    <t>Intersectings</t>
-  </si>
-  <si>
-    <t>Containinigs</t>
   </si>
   <si>
     <t>Polygon Contour</t>
@@ -107,6 +102,15 @@
   <si>
     <t>Elliptical Arc</t>
   </si>
+  <si>
+    <t>Contains</t>
+  </si>
+  <si>
+    <t>Intersects</t>
+  </si>
+  <si>
+    <t>Intersection</t>
+  </si>
 </sst>
 </file>
 
@@ -121,9 +125,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="4" tint="0.59999389629810485"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,17 +152,219 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
@@ -171,11 +376,16 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCECFF"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G16" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G16" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A1:G16">
     <filterColumn colId="6"/>
   </autoFilter>
@@ -186,17 +396,31 @@
     <tableColumn id="4" name="NearestToPoint"/>
     <tableColumn id="5" name="Interpolation"/>
     <tableColumn id="6" name="Length"/>
-    <tableColumn id="7" name="Containinigs"/>
+    <tableColumn id="7" name="Contains"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:P16" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:C16" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A1:C16">
+    <filterColumn colId="2"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Contains"/>
+    <tableColumn id="2" name="Point"/>
+    <tableColumn id="3" name="Rectangle"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:P16" totalsRowShown="0" headerRowDxfId="16">
   <autoFilter ref="A1:P16"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="Intersectings"/>
+    <tableColumn id="1" name="Intersects"/>
     <tableColumn id="2" name="Point"/>
     <tableColumn id="5" name="Line Segment"/>
     <tableColumn id="3" name="Ray"/>
@@ -204,12 +428,12 @@
     <tableColumn id="12" name="Quadratic Bezier"/>
     <tableColumn id="13" name="Cubic Bezier"/>
     <tableColumn id="6" name="Triangle"/>
+    <tableColumn id="7" name="Rectangle"/>
+    <tableColumn id="14" name="Polygon Contour"/>
     <tableColumn id="8" name="Circle"/>
     <tableColumn id="9" name="Circular Arc"/>
     <tableColumn id="10" name="Ellipse"/>
     <tableColumn id="11" name="Elliptical Arc"/>
-    <tableColumn id="7" name="Rectangle"/>
-    <tableColumn id="14" name="Polygon Contour"/>
     <tableColumn id="15" name="Polyline"/>
     <tableColumn id="16" name="Path"/>
   </tableColumns>
@@ -217,26 +441,26 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:P16" totalsRowShown="0" headerRowDxfId="0">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:P16" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A1:P16"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="Intersections"/>
-    <tableColumn id="2" name="Point"/>
-    <tableColumn id="4" name="Line"/>
-    <tableColumn id="3" name="Ray"/>
-    <tableColumn id="5" name="LineSegment"/>
-    <tableColumn id="6" name="Triangle"/>
-    <tableColumn id="7" name="Rectangle"/>
-    <tableColumn id="8" name="Circle"/>
-    <tableColumn id="9" name="CircularArc"/>
-    <tableColumn id="10" name="Ellipse"/>
-    <tableColumn id="11" name="EllipticalArc"/>
-    <tableColumn id="12" name="QuadraticBezier"/>
-    <tableColumn id="13" name="CubicBezier"/>
-    <tableColumn id="14" name="Polygon"/>
-    <tableColumn id="15" name="Polyline"/>
-    <tableColumn id="16" name="Path"/>
+    <tableColumn id="1" name="Intersection"/>
+    <tableColumn id="2" name="Point" dataDxfId="14"/>
+    <tableColumn id="5" name="Line Segment" dataDxfId="13"/>
+    <tableColumn id="3" name="Ray" dataDxfId="12"/>
+    <tableColumn id="4" name="Line" dataDxfId="11"/>
+    <tableColumn id="12" name="Quadratic Bezier" dataDxfId="10"/>
+    <tableColumn id="13" name="Cubic Bezier" dataDxfId="9"/>
+    <tableColumn id="6" name="Triangle" dataDxfId="8"/>
+    <tableColumn id="7" name="Rectangle" dataDxfId="7"/>
+    <tableColumn id="14" name="Polygon Contour" dataDxfId="6"/>
+    <tableColumn id="8" name="Circle" dataDxfId="5"/>
+    <tableColumn id="9" name="CircularArc" dataDxfId="4"/>
+    <tableColumn id="10" name="Ellipse" dataDxfId="3"/>
+    <tableColumn id="11" name="EllipticalArc" dataDxfId="2"/>
+    <tableColumn id="15" name="Polyline" dataDxfId="1"/>
+    <tableColumn id="16" name="Path" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -530,7 +754,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -541,7 +765,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="63.75">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>15</v>
@@ -559,7 +783,7 @@
         <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -926,169 +1150,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="66.75">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="45">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1096,199 +1203,43 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1296,349 +1247,76 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1648,99 +1326,21 @@
       <c r="C15">
         <v>0</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:P16">
-    <cfRule type="iconSet" priority="10">
+  <conditionalFormatting sqref="B2:C16">
+    <cfRule type="iconSet" priority="2">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1760,58 +1360,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="65.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="66.75">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>14</v>
@@ -1828,13 +1426,13 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1872,10 +1470,10 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1971,11 +1569,11 @@
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
+      <c r="A5" t="s">
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1993,22 +1591,22 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -2022,7 +1620,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2072,7 +1670,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2122,7 +1720,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2134,7 +1732,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -2143,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -2172,7 +1770,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2196,7 +1794,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -2222,158 +1820,158 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="B13">
         <v>0</v>
       </c>
@@ -2384,7 +1982,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -2422,7 +2020,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2572,7 +2170,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:P16">
-    <cfRule type="iconSet" priority="2">
+    <cfRule type="iconSet" priority="14">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -2586,4 +2184,872 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="3" customFormat="1" ht="87" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4">
+        <v>0</v>
+      </c>
+      <c r="P2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1</v>
+      </c>
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
+      <c r="N3" s="4">
+        <v>1</v>
+      </c>
+      <c r="O3" s="4">
+        <v>0</v>
+      </c>
+      <c r="P3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1</v>
+      </c>
+      <c r="N4" s="4">
+        <v>1</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1</v>
+      </c>
+      <c r="M5" s="4">
+        <v>1</v>
+      </c>
+      <c r="N5" s="4">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4">
+        <v>0</v>
+      </c>
+      <c r="P6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <v>0</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4">
+        <v>1</v>
+      </c>
+      <c r="K9" s="4">
+        <v>1</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1</v>
+      </c>
+      <c r="J10" s="4">
+        <v>1</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0</v>
+      </c>
+      <c r="P10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11" s="4">
+        <v>1</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0</v>
+      </c>
+      <c r="P11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
+      <c r="O12" s="4">
+        <v>0</v>
+      </c>
+      <c r="P12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4">
+        <v>1</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1</v>
+      </c>
+      <c r="J13" s="4">
+        <v>1</v>
+      </c>
+      <c r="K13" s="4">
+        <v>1</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0</v>
+      </c>
+      <c r="P14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0</v>
+      </c>
+      <c r="P15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0</v>
+      </c>
+      <c r="P16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:P16">
+    <cfRule type="iconSet" priority="11">
+      <iconSet iconSet="3Symbols2">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating to latest VS Preview
Updating Intersection table.
Updating to latest pre-release of Visual Studio.
Updating .NET Framework to 4.7.1.
Updating Nuget Packages to latest.
Isolating Text object from GDI, and providing platform plug for
measurements.
Movine more objects from Winforms shim to main Engine.
</commit_message>
<xml_diff>
--- a/Documents/Geometry.xlsx
+++ b/Documents/Geometry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19155" windowHeight="7245" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19155" windowHeight="7245" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="3" r:id="rId1"/>
@@ -169,7 +169,11 @@
   <dxfs count="19">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -182,7 +186,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -195,7 +203,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -208,7 +220,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -422,19 +438,19 @@
   <tableColumns count="16">
     <tableColumn id="1" name="Intersects"/>
     <tableColumn id="2" name="Point"/>
+    <tableColumn id="4" name="Line"/>
+    <tableColumn id="3" name="Ray"/>
     <tableColumn id="5" name="Line Segment"/>
-    <tableColumn id="3" name="Ray"/>
-    <tableColumn id="4" name="Line"/>
     <tableColumn id="12" name="Quadratic Bezier"/>
     <tableColumn id="13" name="Cubic Bezier"/>
     <tableColumn id="6" name="Triangle"/>
     <tableColumn id="7" name="Rectangle"/>
+    <tableColumn id="15" name="Polyline"/>
     <tableColumn id="14" name="Polygon Contour"/>
     <tableColumn id="8" name="Circle"/>
     <tableColumn id="9" name="Circular Arc"/>
     <tableColumn id="10" name="Ellipse"/>
     <tableColumn id="11" name="Elliptical Arc"/>
-    <tableColumn id="15" name="Polyline"/>
     <tableColumn id="16" name="Path"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -447,20 +463,20 @@
   <tableColumns count="16">
     <tableColumn id="1" name="Intersection"/>
     <tableColumn id="2" name="Point" dataDxfId="14"/>
+    <tableColumn id="4" name="Line" dataDxfId="2"/>
+    <tableColumn id="3" name="Ray" dataDxfId="1"/>
     <tableColumn id="5" name="Line Segment" dataDxfId="13"/>
-    <tableColumn id="3" name="Ray" dataDxfId="12"/>
-    <tableColumn id="4" name="Line" dataDxfId="11"/>
-    <tableColumn id="12" name="Quadratic Bezier" dataDxfId="10"/>
-    <tableColumn id="13" name="Cubic Bezier" dataDxfId="9"/>
-    <tableColumn id="6" name="Triangle" dataDxfId="8"/>
-    <tableColumn id="7" name="Rectangle" dataDxfId="7"/>
-    <tableColumn id="14" name="Polygon Contour" dataDxfId="6"/>
-    <tableColumn id="8" name="Circle" dataDxfId="5"/>
-    <tableColumn id="9" name="CircularArc" dataDxfId="4"/>
-    <tableColumn id="10" name="Ellipse" dataDxfId="3"/>
-    <tableColumn id="11" name="EllipticalArc" dataDxfId="2"/>
-    <tableColumn id="15" name="Polyline" dataDxfId="1"/>
-    <tableColumn id="16" name="Path" dataDxfId="0"/>
+    <tableColumn id="12" name="Quadratic Bezier" dataDxfId="3"/>
+    <tableColumn id="13" name="Cubic Bezier" dataDxfId="12"/>
+    <tableColumn id="6" name="Triangle" dataDxfId="11"/>
+    <tableColumn id="7" name="Rectangle" dataDxfId="10"/>
+    <tableColumn id="15" name="Polyline" dataDxfId="0"/>
+    <tableColumn id="14" name="Polygon Contour" dataDxfId="9"/>
+    <tableColumn id="8" name="Circle" dataDxfId="8"/>
+    <tableColumn id="9" name="CircularArc" dataDxfId="7"/>
+    <tableColumn id="10" name="Ellipse" dataDxfId="6"/>
+    <tableColumn id="11" name="EllipticalArc" dataDxfId="5"/>
+    <tableColumn id="16" name="Path" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1360,7 +1376,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1376,13 +1394,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>22</v>
@@ -1397,22 +1415,22 @@
         <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>12</v>
@@ -1426,13 +1444,13 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1470,10 +1488,10 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1570,10 +1588,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1820,7 +1838,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1870,7 +1888,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1900,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1920,7 +1938,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1953,7 +1971,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1970,7 +1988,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -2020,7 +2038,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2070,7 +2088,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2170,7 +2188,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:P16">
-    <cfRule type="iconSet" priority="14">
+    <cfRule type="iconSet" priority="20">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -2190,8 +2208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2208,13 +2226,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>22</v>
@@ -2229,22 +2247,22 @@
         <v>2</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>12</v>
@@ -2302,7 +2320,7 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -2329,7 +2347,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" s="4">
         <v>1</v>
@@ -2344,7 +2362,7 @@
         <v>1</v>
       </c>
       <c r="O3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" s="4">
         <v>0</v>
@@ -2379,7 +2397,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="4">
         <v>1</v>
@@ -2394,7 +2412,7 @@
         <v>1</v>
       </c>
       <c r="O4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="4">
         <v>0</v>
@@ -2402,7 +2420,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
@@ -2429,7 +2447,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="4">
         <v>1</v>
@@ -2444,7 +2462,7 @@
         <v>1</v>
       </c>
       <c r="O5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" s="4">
         <v>0</v>
@@ -2479,19 +2497,19 @@
         <v>1</v>
       </c>
       <c r="J6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="4">
         <v>1</v>
       </c>
       <c r="L6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" s="4">
         <v>0</v>
@@ -2529,19 +2547,19 @@
         <v>1</v>
       </c>
       <c r="J7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="4">
         <v>1</v>
       </c>
       <c r="L7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" s="4">
         <v>0</v>
@@ -2579,19 +2597,19 @@
         <v>1</v>
       </c>
       <c r="J8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" s="4">
         <v>1</v>
       </c>
       <c r="L8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8" s="4">
         <v>0</v>
@@ -2629,19 +2647,19 @@
         <v>1</v>
       </c>
       <c r="J9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" s="4">
         <v>1</v>
       </c>
       <c r="L9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" s="4">
         <v>0</v>
@@ -2652,43 +2670,43 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B10" s="4">
         <v>0</v>
       </c>
       <c r="C10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" s="4">
         <v>0</v>
       </c>
       <c r="M10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" s="4">
         <v>0</v>
@@ -2702,7 +2720,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4">
         <v>0</v>
@@ -2729,19 +2747,19 @@
         <v>1</v>
       </c>
       <c r="J11" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="4">
         <v>1</v>
       </c>
       <c r="L11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" s="4">
         <v>0</v>
@@ -2752,7 +2770,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="4">
         <v>0</v>
@@ -2767,31 +2785,31 @@
         <v>1</v>
       </c>
       <c r="F12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="4">
         <v>0</v>
       </c>
       <c r="K12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="4">
         <v>0</v>
       </c>
       <c r="N12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12" s="4">
         <v>0</v>
@@ -2802,119 +2820,119 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="4">
-        <v>0</v>
-      </c>
-      <c r="C13" s="4">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-      <c r="G13" s="4">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4">
-        <v>1</v>
-      </c>
-      <c r="I13" s="4">
-        <v>1</v>
-      </c>
-      <c r="J13" s="4">
-        <v>1</v>
-      </c>
-      <c r="K13" s="4">
-        <v>1</v>
-      </c>
-      <c r="L13" s="4">
-        <v>0</v>
-      </c>
-      <c r="M13" s="4">
-        <v>1</v>
-      </c>
-      <c r="N13" s="4">
-        <v>0</v>
-      </c>
-      <c r="O13" s="4">
-        <v>0</v>
-      </c>
-      <c r="P13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1</v>
+      </c>
+      <c r="L14" s="4">
+        <v>1</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>1</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0</v>
+      </c>
+      <c r="P14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="4">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4">
-        <v>0</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0</v>
-      </c>
-      <c r="H14" s="4">
-        <v>0</v>
-      </c>
-      <c r="I14" s="4">
-        <v>0</v>
-      </c>
-      <c r="J14" s="4">
-        <v>0</v>
-      </c>
-      <c r="K14" s="4">
-        <v>0</v>
-      </c>
-      <c r="L14" s="4">
-        <v>0</v>
-      </c>
-      <c r="M14" s="4">
-        <v>0</v>
-      </c>
-      <c r="N14" s="4">
-        <v>0</v>
-      </c>
-      <c r="O14" s="4">
-        <v>0</v>
-      </c>
-      <c r="P14" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
       <c r="B15" s="4">
         <v>0</v>
       </c>
       <c r="C15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="4">
         <v>0</v>
@@ -3002,7 +3020,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:P16">
-    <cfRule type="iconSet" priority="11">
+    <cfRule type="iconSet" priority="20">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>

</xml_diff>

<commit_message>
Trying to Figure out Rotated Ellipse Bezier Intersection
Work trying to figure out how to find the intersections between rotated ellipses and Bezier curves. Not close to getting it to work yet.
Updating to latest .NET.
Updating to latest Visual Studio preview.
</commit_message>
<xml_diff>
--- a/Documents/Geometry.xlsx
+++ b/Documents/Geometry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19155" windowHeight="7245" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19155" windowHeight="7245" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="35">
   <si>
     <t>Point</t>
   </si>
@@ -110,13 +110,28 @@
   </si>
   <si>
     <t>Intersection</t>
+  </si>
+  <si>
+    <t>Rotated Ellipse</t>
+  </si>
+  <si>
+    <t>Orthogonal Ellipse</t>
+  </si>
+  <si>
+    <t>Rotated Elliptical Arc</t>
+  </si>
+  <si>
+    <t>Orthogonal Elliptical Arc</t>
+  </si>
+  <si>
+    <t>Orthogonal EllipticalArc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +144,12 @@
       <color theme="4" tint="0.59999389629810485"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -152,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -162,45 +183,12 @@
       <alignment horizontal="left" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="4" tint="0.59999389629810485"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="4" tint="0.59999389629810485"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <font>
         <b val="0"/>
@@ -315,7 +303,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -367,6 +359,70 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -401,7 +457,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G16" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G16" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="A1:G16">
     <filterColumn colId="6"/>
   </autoFilter>
@@ -419,7 +475,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:C16" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:C16" totalsRowShown="0" headerRowDxfId="19">
   <autoFilter ref="A1:C16">
     <filterColumn colId="2"/>
   </autoFilter>
@@ -433,7 +489,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:P16" totalsRowShown="0" headerRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:P16" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A1:P16"/>
   <tableColumns count="16">
     <tableColumn id="1" name="Intersects"/>
@@ -458,25 +514,30 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:P16" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A1:P16"/>
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:R18" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A1:R18">
+    <filterColumn colId="14"/>
+    <filterColumn colId="16"/>
+  </autoFilter>
+  <tableColumns count="18">
     <tableColumn id="1" name="Intersection"/>
-    <tableColumn id="2" name="Point" dataDxfId="14"/>
-    <tableColumn id="4" name="Line" dataDxfId="2"/>
-    <tableColumn id="3" name="Ray" dataDxfId="1"/>
+    <tableColumn id="2" name="Point" dataDxfId="16"/>
+    <tableColumn id="4" name="Line" dataDxfId="15"/>
+    <tableColumn id="3" name="Ray" dataDxfId="14"/>
     <tableColumn id="5" name="Line Segment" dataDxfId="13"/>
-    <tableColumn id="12" name="Quadratic Bezier" dataDxfId="3"/>
-    <tableColumn id="13" name="Cubic Bezier" dataDxfId="12"/>
-    <tableColumn id="6" name="Triangle" dataDxfId="11"/>
-    <tableColumn id="7" name="Rectangle" dataDxfId="10"/>
-    <tableColumn id="15" name="Polyline" dataDxfId="0"/>
-    <tableColumn id="14" name="Polygon Contour" dataDxfId="9"/>
-    <tableColumn id="8" name="Circle" dataDxfId="8"/>
-    <tableColumn id="9" name="CircularArc" dataDxfId="7"/>
-    <tableColumn id="10" name="Ellipse" dataDxfId="6"/>
-    <tableColumn id="11" name="EllipticalArc" dataDxfId="5"/>
-    <tableColumn id="16" name="Path" dataDxfId="4"/>
+    <tableColumn id="12" name="Quadratic Bezier" dataDxfId="12"/>
+    <tableColumn id="13" name="Cubic Bezier" dataDxfId="11"/>
+    <tableColumn id="6" name="Triangle" dataDxfId="10"/>
+    <tableColumn id="7" name="Rectangle" dataDxfId="9"/>
+    <tableColumn id="15" name="Polyline" dataDxfId="8"/>
+    <tableColumn id="14" name="Polygon Contour" dataDxfId="7"/>
+    <tableColumn id="8" name="Circle" dataDxfId="6"/>
+    <tableColumn id="9" name="CircularArc" dataDxfId="5"/>
+    <tableColumn id="10" name="Orthogonal Ellipse" dataDxfId="4"/>
+    <tableColumn id="17" name="Rotated Ellipse" dataDxfId="1"/>
+    <tableColumn id="11" name="Orthogonal EllipticalArc" dataDxfId="3"/>
+    <tableColumn id="18" name="Rotated Elliptical Arc" dataDxfId="0"/>
+    <tableColumn id="16" name="Path" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1376,7 +1437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -2206,19 +2267,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.28515625" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.28515625" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" ht="87" customHeight="1">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="87" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -2259,16 +2322,22 @@
         <v>7</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="P1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2291,16 +2360,16 @@
         <v>0</v>
       </c>
       <c r="H2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" s="4">
         <v>0</v>
@@ -2317,8 +2386,14 @@
       <c r="P2" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2" s="4">
+        <v>0</v>
+      </c>
+      <c r="R2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2347,7 +2422,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="4">
         <v>1</v>
@@ -2365,10 +2440,16 @@
         <v>1</v>
       </c>
       <c r="P3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>0</v>
+      </c>
+      <c r="R3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -2397,7 +2478,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="4">
         <v>1</v>
@@ -2415,10 +2496,16 @@
         <v>1</v>
       </c>
       <c r="P4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>0</v>
+      </c>
+      <c r="R4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -2447,7 +2534,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="4">
         <v>1</v>
@@ -2465,10 +2552,16 @@
         <v>1</v>
       </c>
       <c r="P5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>0</v>
+      </c>
+      <c r="R5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2497,7 +2590,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="4">
         <v>1</v>
@@ -2517,8 +2610,14 @@
       <c r="P6" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="Q6" s="4">
+        <v>0</v>
+      </c>
+      <c r="R6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2547,7 +2646,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="4">
         <v>1</v>
@@ -2567,13 +2666,19 @@
       <c r="P7" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="Q7" s="4">
+        <v>0</v>
+      </c>
+      <c r="R7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -2597,7 +2702,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="4">
         <v>1</v>
@@ -2612,18 +2717,24 @@
         <v>1</v>
       </c>
       <c r="O8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="Q8" s="4">
+        <v>0</v>
+      </c>
+      <c r="R8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -2647,7 +2758,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="4">
         <v>1</v>
@@ -2662,68 +2773,80 @@
         <v>1</v>
       </c>
       <c r="O9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="Q9" s="4">
+        <v>0</v>
+      </c>
+      <c r="R9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="4">
         <v>0</v>
       </c>
       <c r="N10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="Q10" s="4">
+        <v>0</v>
+      </c>
+      <c r="R10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -2747,7 +2870,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="4">
         <v>1</v>
@@ -2762,13 +2885,19 @@
         <v>1</v>
       </c>
       <c r="O11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="Q11" s="4">
+        <v>0</v>
+      </c>
+      <c r="R11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -2797,7 +2926,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="4">
         <v>1</v>
@@ -2812,13 +2941,19 @@
         <v>1</v>
       </c>
       <c r="O12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="Q12" s="4">
+        <v>0</v>
+      </c>
+      <c r="R12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -2867,10 +3002,16 @@
       <c r="P13" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="Q13" s="4">
+        <v>0</v>
+      </c>
+      <c r="R13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B14" s="4">
         <v>0</v>
@@ -2897,7 +3038,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="4">
         <v>1</v>
@@ -2912,114 +3053,244 @@
         <v>1</v>
       </c>
       <c r="O14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="4">
-        <v>0</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0</v>
-      </c>
-      <c r="I15" s="4">
-        <v>0</v>
-      </c>
-      <c r="J15" s="4">
-        <v>0</v>
-      </c>
-      <c r="K15" s="4">
-        <v>0</v>
-      </c>
-      <c r="L15" s="4">
-        <v>0</v>
-      </c>
-      <c r="M15" s="4">
-        <v>0</v>
-      </c>
-      <c r="N15" s="4">
-        <v>0</v>
-      </c>
-      <c r="O15" s="4">
-        <v>0</v>
-      </c>
-      <c r="P15" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="Q14" s="4">
+        <v>0</v>
+      </c>
+      <c r="R14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5">
+        <v>1</v>
+      </c>
+      <c r="J15" s="5">
+        <v>1</v>
+      </c>
+      <c r="K15" s="5">
+        <v>1</v>
+      </c>
+      <c r="L15" s="5">
+        <v>1</v>
+      </c>
+      <c r="M15" s="5">
+        <v>0</v>
+      </c>
+      <c r="N15" s="5">
+        <v>1</v>
+      </c>
+      <c r="O15" s="5">
+        <v>1</v>
+      </c>
+      <c r="P15" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>0</v>
+      </c>
+      <c r="R15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0</v>
+      </c>
+      <c r="P16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>0</v>
+      </c>
+      <c r="R16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0</v>
+      </c>
+      <c r="K17" s="5">
+        <v>0</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0</v>
+      </c>
+      <c r="M17" s="5">
+        <v>0</v>
+      </c>
+      <c r="N17" s="5">
+        <v>0</v>
+      </c>
+      <c r="O17" s="5">
+        <v>0</v>
+      </c>
+      <c r="P17" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>0</v>
+      </c>
+      <c r="R17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="4">
-        <v>0</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
-        <v>0</v>
-      </c>
-      <c r="K16" s="4">
-        <v>0</v>
-      </c>
-      <c r="L16" s="4">
-        <v>0</v>
-      </c>
-      <c r="M16" s="4">
-        <v>0</v>
-      </c>
-      <c r="N16" s="4">
-        <v>0</v>
-      </c>
-      <c r="O16" s="4">
-        <v>0</v>
-      </c>
-      <c r="P16" s="4">
+      <c r="B18" s="4">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0</v>
+      </c>
+      <c r="O18" s="4">
+        <v>0</v>
+      </c>
+      <c r="P18" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>0</v>
+      </c>
+      <c r="R18" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:P16">
+  <conditionalFormatting sqref="B2:R18">
     <cfRule type="iconSet" priority="20">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>

</xml_diff>

<commit_message>
More Ellipse intersection fixes
Fixing some cases where intersections between oblique ellipses were failing.
</commit_message>
<xml_diff>
--- a/Documents/Geometry.xlsx
+++ b/Documents/Geometry.xlsx
@@ -112,19 +112,19 @@
     <t>Intersection</t>
   </si>
   <si>
-    <t>Rotated Ellipse</t>
-  </si>
-  <si>
     <t>Orthogonal Ellipse</t>
   </si>
   <si>
-    <t>Rotated Elliptical Arc</t>
-  </si>
-  <si>
     <t>Orthogonal Elliptical Arc</t>
   </si>
   <si>
     <t>Orthogonal EllipticalArc</t>
+  </si>
+  <si>
+    <t>Oblique Ellipse</t>
+  </si>
+  <si>
+    <t>Oblique Elliptical Arc</t>
   </si>
 </sst>
 </file>
@@ -191,11 +191,7 @@
   <dxfs count="21">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -238,7 +234,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -534,10 +534,10 @@
     <tableColumn id="8" name="Circle" dataDxfId="6"/>
     <tableColumn id="9" name="CircularArc" dataDxfId="5"/>
     <tableColumn id="10" name="Orthogonal Ellipse" dataDxfId="4"/>
-    <tableColumn id="17" name="Rotated Ellipse" dataDxfId="1"/>
-    <tableColumn id="11" name="Orthogonal EllipticalArc" dataDxfId="3"/>
-    <tableColumn id="18" name="Rotated Elliptical Arc" dataDxfId="0"/>
-    <tableColumn id="16" name="Path" dataDxfId="2"/>
+    <tableColumn id="17" name="Oblique Ellipse" dataDxfId="3"/>
+    <tableColumn id="11" name="Orthogonal EllipticalArc" dataDxfId="2"/>
+    <tableColumn id="18" name="Oblique Elliptical Arc" dataDxfId="1"/>
+    <tableColumn id="16" name="Path" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2269,7 +2269,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2322,16 +2324,16 @@
         <v>7</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="P1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>12</v>
@@ -2605,7 +2607,7 @@
         <v>1</v>
       </c>
       <c r="O6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" s="4">
         <v>0</v>
@@ -2661,7 +2663,7 @@
         <v>1</v>
       </c>
       <c r="O7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" s="4">
         <v>0</v>
@@ -3011,7 +3013,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="4">
         <v>0</v>
@@ -3067,7 +3069,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B15" s="5">
         <v>0</v>
@@ -3082,10 +3084,10 @@
         <v>1</v>
       </c>
       <c r="F15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <v>1</v>
@@ -3123,7 +3125,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="4">
         <v>0</v>
@@ -3179,7 +3181,7 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B17" s="5">
         <v>0</v>

</xml_diff>